<commit_message>
Removed hard coded data for the products tests
</commit_message>
<xml_diff>
--- a/selenium-based-ui-automation/src/test/resources/test-data/sit-test-data.xlsx
+++ b/selenium-based-ui-automation/src/test/resources/test-data/sit-test-data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\baji0\eclipse-workspace\selenium-based-ui-automation\src\test\resources\test-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\baji0\git\selenium-java-testng-framework\selenium-based-ui-automation\src\test\resources\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD9ABD67-32BE-489A-A1C1-070AB4677117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F4D0338-9CE6-4E73-8605-CA921D91C1BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>TC_001</t>
   </si>
@@ -125,6 +125,21 @@
   </si>
   <si>
     <t>Name (A to Z)</t>
+  </si>
+  <si>
+    <t>TC_009</t>
+  </si>
+  <si>
+    <t>TC_010</t>
+  </si>
+  <si>
+    <t>Sauce Labs Backpack, Sauce Labs Bike Light, Sauce Labs Bolt T-Shirt, Sauce Labs Fleece Jacket, Sauce Labs Onesie, Test.allTheThings() T-Shirt (Red)</t>
+  </si>
+  <si>
+    <t>Test.allTheThings() T-Shirt (Red), Sauce Labs Onesie, Sauce Labs Fleece Jacket, Sauce Labs Bolt T-Shirt, Sauce Labs Bike Light, Sauce Labs Backpack</t>
+  </si>
+  <si>
+    <t>Name (A to Z), Name (Z to A), Price (low to high), Price (high to low)</t>
   </si>
 </sst>
 </file>
@@ -160,8 +175,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -550,24 +568,44 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC98A5B7-1B07-4BC7-A086-0DF4ECB7EA35}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.109375" customWidth="1"/>
-    <col min="2" max="2" width="31.21875" customWidth="1"/>
+    <col min="2" max="2" width="56.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="78.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1235431</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added few products tests to the suite
</commit_message>
<xml_diff>
--- a/selenium-based-ui-automation/src/test/resources/test-data/sit-test-data.xlsx
+++ b/selenium-based-ui-automation/src/test/resources/test-data/sit-test-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\baji0\git\selenium-java-testng-framework\selenium-based-ui-automation\src\test\resources\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F4D0338-9CE6-4E73-8605-CA921D91C1BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BA1339-291F-466F-9B93-77543D7D2A25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>TC_001</t>
   </si>
@@ -140,6 +140,18 @@
   </si>
   <si>
     <t>Name (A to Z), Name (Z to A), Price (low to high), Price (high to low)</t>
+  </si>
+  <si>
+    <t>TC_011</t>
+  </si>
+  <si>
+    <t>7.99, 9.99, 15.99, 15.99, 29.99, 49.99</t>
+  </si>
+  <si>
+    <t>TC_012</t>
+  </si>
+  <si>
+    <t>49.99, 29.99, 15.99, 15.99, 9.99, 7.99</t>
   </si>
 </sst>
 </file>
@@ -568,10 +580,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC98A5B7-1B07-4BC7-A086-0DF4ECB7EA35}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -608,6 +620,22 @@
         <v>16</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>